<commit_message>
SleepTrack V3 Artwork Rev B
-Updated Artwork to connect USB pin 5 to GND instead of Dummy NEt
-Removed Vout+ and NC trace
-Regenerated manufacture files and PDFs
</commit_message>
<xml_diff>
--- a/Photon_Dev/Bill of Materials/BOM.xlsx
+++ b/Photon_Dev/Bill of Materials/BOM.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27870" windowHeight="13020"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27870" windowHeight="13020" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PROTON_DEV" sheetId="1" r:id="rId1"/>
@@ -674,7 +674,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -833,107 +833,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -998,7 +897,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1035,37 +934,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="45">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1395,8 +1264,8 @@
   </sheetPr>
   <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection sqref="A1:D49"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1459,7 +1328,7 @@
     </row>
     <row r="10" spans="1:8" ht="15.75" thickBot="1"/>
     <row r="11" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A11" s="26" t="s">
+      <c r="A11" s="16" t="s">
         <v>0</v>
       </c>
       <c r="B11" s="11" t="s">
@@ -2404,8 +2273,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2417,7 +2286,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
@@ -2431,7 +2300,7 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="16">
+      <c r="A2" s="9">
         <v>1</v>
       </c>
       <c r="B2" s="9">
@@ -2440,12 +2309,12 @@
       <c r="C2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="9" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="18">
+      <c r="A3" s="5">
         <v>2</v>
       </c>
       <c r="B3" s="5">
@@ -2454,12 +2323,12 @@
       <c r="C3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="18">
+      <c r="A4" s="5">
         <v>3</v>
       </c>
       <c r="B4" s="5">
@@ -2468,12 +2337,12 @@
       <c r="C4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="5" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="18">
+      <c r="A5" s="5">
         <v>4</v>
       </c>
       <c r="B5" s="5">
@@ -2482,12 +2351,12 @@
       <c r="C5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="5" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="45">
-      <c r="A6" s="18">
+      <c r="A6" s="5">
         <v>5</v>
       </c>
       <c r="B6" s="5">
@@ -2496,12 +2365,12 @@
       <c r="C6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="7" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="18">
+      <c r="A7" s="5">
         <v>6</v>
       </c>
       <c r="B7" s="5">
@@ -2510,12 +2379,12 @@
       <c r="C7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="5" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="18">
+      <c r="A8" s="5">
         <v>7</v>
       </c>
       <c r="B8" s="5">
@@ -2524,12 +2393,12 @@
       <c r="C8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="5" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="18">
+      <c r="A9" s="5">
         <v>9</v>
       </c>
       <c r="B9" s="5">
@@ -2538,12 +2407,12 @@
       <c r="C9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="5" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="18">
+      <c r="A10" s="5">
         <v>10</v>
       </c>
       <c r="B10" s="5">
@@ -2552,12 +2421,12 @@
       <c r="C10" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="D10" s="5" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="18">
+      <c r="A11" s="5">
         <v>11</v>
       </c>
       <c r="B11" s="5">
@@ -2566,12 +2435,12 @@
       <c r="C11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="5" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="18">
+      <c r="A12" s="5">
         <v>12</v>
       </c>
       <c r="B12" s="5">
@@ -2580,12 +2449,12 @@
       <c r="C12" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="19" t="s">
+      <c r="D12" s="5" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="18">
+      <c r="A13" s="5">
         <v>13</v>
       </c>
       <c r="B13" s="5">
@@ -2594,12 +2463,12 @@
       <c r="C13" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="D13" s="5" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="30">
-      <c r="A14" s="18">
+      <c r="A14" s="5">
         <v>14</v>
       </c>
       <c r="B14" s="5">
@@ -2608,12 +2477,12 @@
       <c r="C14" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="20" t="s">
+      <c r="D14" s="7" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="18">
+      <c r="A15" s="5">
         <v>15</v>
       </c>
       <c r="B15" s="5">
@@ -2622,12 +2491,12 @@
       <c r="C15" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="5" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="18">
+      <c r="A16" s="5">
         <v>16</v>
       </c>
       <c r="B16" s="5">
@@ -2636,12 +2505,12 @@
       <c r="C16" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="19" t="s">
+      <c r="D16" s="5" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="18">
+      <c r="A17" s="5">
         <v>17</v>
       </c>
       <c r="B17" s="5">
@@ -2650,12 +2519,12 @@
       <c r="C17" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="19" t="s">
+      <c r="D17" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="18">
+      <c r="A18" s="5">
         <v>18</v>
       </c>
       <c r="B18" s="5">
@@ -2664,12 +2533,12 @@
       <c r="C18" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D18" s="19" t="s">
+      <c r="D18" s="5" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="18">
+      <c r="A19" s="5">
         <v>19</v>
       </c>
       <c r="B19" s="5">
@@ -2678,12 +2547,12 @@
       <c r="C19" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="19" t="s">
+      <c r="D19" s="5" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="18">
+      <c r="A20" s="5">
         <v>20</v>
       </c>
       <c r="B20" s="5">
@@ -2692,12 +2561,12 @@
       <c r="C20" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D20" s="19" t="s">
+      <c r="D20" s="5" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="18">
+      <c r="A21" s="5">
         <v>21</v>
       </c>
       <c r="B21" s="5">
@@ -2706,12 +2575,12 @@
       <c r="C21" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D21" s="19" t="s">
+      <c r="D21" s="5" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="18">
+      <c r="A22" s="5">
         <v>22</v>
       </c>
       <c r="B22" s="5">
@@ -2720,12 +2589,12 @@
       <c r="C22" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D22" s="19" t="s">
+      <c r="D22" s="5" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="18">
+      <c r="A23" s="5">
         <v>23</v>
       </c>
       <c r="B23" s="5">
@@ -2734,12 +2603,12 @@
       <c r="C23" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D23" s="19" t="s">
+      <c r="D23" s="5" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="18">
+      <c r="A24" s="5">
         <v>24</v>
       </c>
       <c r="B24" s="5">
@@ -2748,12 +2617,12 @@
       <c r="C24" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D24" s="19" t="s">
+      <c r="D24" s="5" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="18">
+      <c r="A25" s="5">
         <v>25</v>
       </c>
       <c r="B25" s="5">
@@ -2762,12 +2631,12 @@
       <c r="C25" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D25" s="19" t="s">
+      <c r="D25" s="5" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="18">
+      <c r="A26" s="5">
         <v>26</v>
       </c>
       <c r="B26" s="5">
@@ -2776,12 +2645,12 @@
       <c r="C26" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D26" s="19" t="s">
+      <c r="D26" s="5" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="18">
+      <c r="A27" s="5">
         <v>27</v>
       </c>
       <c r="B27" s="5">
@@ -2790,12 +2659,12 @@
       <c r="C27" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D27" s="19" t="s">
+      <c r="D27" s="5" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="18">
+      <c r="A28" s="5">
         <v>28</v>
       </c>
       <c r="B28" s="5">
@@ -2804,12 +2673,12 @@
       <c r="C28" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D28" s="19" t="s">
+      <c r="D28" s="5" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="18">
+      <c r="A29" s="5">
         <v>29</v>
       </c>
       <c r="B29" s="5">
@@ -2818,12 +2687,12 @@
       <c r="C29" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D29" s="19" t="s">
+      <c r="D29" s="5" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="18">
+      <c r="A30" s="5">
         <v>30</v>
       </c>
       <c r="B30" s="5">
@@ -2832,12 +2701,12 @@
       <c r="C30" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="D30" s="19" t="s">
+      <c r="D30" s="5" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="18">
+      <c r="A31" s="5">
         <v>31</v>
       </c>
       <c r="B31" s="5">
@@ -2846,12 +2715,12 @@
       <c r="C31" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D31" s="19" t="s">
+      <c r="D31" s="5" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:4">
-      <c r="A32" s="18">
+      <c r="A32" s="5">
         <v>32</v>
       </c>
       <c r="B32" s="5">
@@ -2860,12 +2729,12 @@
       <c r="C32" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D32" s="19" t="s">
+      <c r="D32" s="5" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33" s="18">
+      <c r="A33" s="5">
         <v>34</v>
       </c>
       <c r="B33" s="5">
@@ -2874,12 +2743,12 @@
       <c r="C33" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D33" s="19" t="s">
+      <c r="D33" s="5" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="34" spans="1:4">
-      <c r="A34" s="21">
+      <c r="A34" s="13">
         <v>35</v>
       </c>
       <c r="B34" s="13">
@@ -2888,12 +2757,12 @@
       <c r="C34" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D34" s="22" t="s">
+      <c r="D34" s="13" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35" s="18">
+      <c r="A35" s="5">
         <v>36</v>
       </c>
       <c r="B35" s="5">
@@ -2902,12 +2771,12 @@
       <c r="C35" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D35" s="19" t="s">
+      <c r="D35" s="5" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="36" spans="1:4">
-      <c r="A36" s="18">
+      <c r="A36" s="5">
         <v>37</v>
       </c>
       <c r="B36" s="5">
@@ -2916,12 +2785,12 @@
       <c r="C36" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D36" s="19" t="s">
+      <c r="D36" s="5" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="18">
+      <c r="A37" s="5">
         <v>38</v>
       </c>
       <c r="B37" s="5">
@@ -2930,12 +2799,12 @@
       <c r="C37" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D37" s="19" t="s">
+      <c r="D37" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" s="18">
+      <c r="A38" s="5">
         <v>39</v>
       </c>
       <c r="B38" s="5">
@@ -2944,21 +2813,21 @@
       <c r="C38" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D38" s="19" t="s">
+      <c r="D38" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A39" s="23">
+    <row r="39" spans="1:4">
+      <c r="A39" s="5">
         <v>40</v>
       </c>
-      <c r="B39" s="24">
-        <v>1</v>
-      </c>
-      <c r="C39" s="24" t="s">
+      <c r="B39" s="5">
+        <v>1</v>
+      </c>
+      <c r="C39" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D39" s="25" t="s">
+      <c r="D39" s="5" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>